<commit_message>
CON MODIFICACIÓN SVG PARA BIPLOT
</commit_message>
<xml_diff>
--- a/Indc WDI_V4.xlsx
+++ b/Indc WDI_V4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\messi\OneDrive\Escritorio\escuela\Servicio Social\Python\PCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AF7D2D8-502D-4D3C-A7CD-04D23A1A2158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB947EE1-8C0C-4013-BBDC-606A1D943742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="11" activeTab="12" xr2:uid="{D86699F4-EEE8-4FD6-B0D7-CE6A5D28E5C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="12" activeTab="14" xr2:uid="{D86699F4-EEE8-4FD6-B0D7-CE6A5D28E5C9}"/>
   </bookViews>
   <sheets>
     <sheet name="GDP growth (annual %)" sheetId="25" r:id="rId1"/>
@@ -223,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -232,7 +232,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8452,7 +8451,7 @@
       <c r="J5">
         <v>3313.5263671875</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <f>N5</f>
         <v>4497.48681640625</v>
       </c>
@@ -10586,8 +10585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D64FC8F-D734-42A8-9038-CF327D7C7E20}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15768,7 +15767,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575C0386-4DAA-4C42-A1EB-06E5AACD93A5}">
   <dimension ref="A1:X35"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -16210,6 +16211,10 @@
       <c r="W6">
         <v>6.3</v>
       </c>
+      <c r="X6" s="5">
+        <f>W6</f>
+        <v>6.3</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -17019,6 +17024,10 @@
         <v>3.11</v>
       </c>
       <c r="W17">
+        <v>3.04</v>
+      </c>
+      <c r="X17" s="5">
+        <f>W17</f>
         <v>3.04</v>
       </c>
     </row>

</xml_diff>